<commit_message>
fixed bug with dynamic data population and edits to README.md
</commit_message>
<xml_diff>
--- a/CalendarEvents.xlsx
+++ b/CalendarEvents.xlsx
@@ -180,7 +180,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +191,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -222,37 +228,49 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -580,15 +598,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="28.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="42.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="68.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="11.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="10" width="13.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="9" width="33.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="28.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="42.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="68.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="13" width="11.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="14" width="13.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="15.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="12" width="12.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="12" width="33.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -601,1022 +619,1022 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="4">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="6">
         <v>45292</v>
       </c>
-      <c r="B2" s="4">
-        <v>99714.49930555555</v>
+      <c r="B2" s="6">
+        <v>45292.49930555555</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="7"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
       <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="4">
+      <c r="H2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="6">
         <v>45293</v>
       </c>
-      <c r="B3" s="4">
-        <v>99715.49930555555</v>
+      <c r="B3" s="6">
+        <v>45293.49930555555</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="9"/>
       <c r="G3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="4">
+      <c r="H3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="6">
         <v>45313</v>
       </c>
-      <c r="B4" s="4">
-        <v>99735.49930555555</v>
+      <c r="B4" s="6">
+        <v>45313.49930555555</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="9"/>
       <c r="G4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="4">
+      <c r="H4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="6">
         <v>45320</v>
       </c>
-      <c r="B5" s="4">
-        <v>99742.49930555555</v>
+      <c r="B5" s="6">
+        <v>45320.49930555555</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9"/>
       <c r="G5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="4">
+      <c r="H5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="6">
         <v>45320</v>
       </c>
-      <c r="B6" s="4">
-        <v>99742.49930555555</v>
+      <c r="B6" s="6">
+        <v>45320.49930555555</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9"/>
       <c r="G6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="4">
+      <c r="H6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="6">
         <v>45317</v>
       </c>
-      <c r="B7" s="4">
-        <v>99739.49930555555</v>
+      <c r="B7" s="6">
+        <v>45317.49930555555</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="9"/>
       <c r="G7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="4">
+      <c r="H7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="6">
         <v>45328</v>
       </c>
-      <c r="B8" s="4">
-        <v>99750.49930555555</v>
+      <c r="B8" s="6">
+        <v>45328.49930555555</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9"/>
       <c r="G8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="4">
+      <c r="H8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="6">
         <v>45355</v>
       </c>
-      <c r="B9" s="4">
-        <v>99776.49930555555</v>
+      <c r="B9" s="6">
+        <v>45355.49930555555</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="7"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9"/>
       <c r="G9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="4">
+      <c r="H9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="6">
         <v>45362</v>
       </c>
-      <c r="B10" s="4">
-        <v>99783.49930555555</v>
+      <c r="B10" s="6">
+        <v>45362.49930555555</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="7"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
       <c r="G10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="4">
+      <c r="H10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="6">
         <v>45362</v>
       </c>
-      <c r="B11" s="4">
-        <v>99783.49930555555</v>
+      <c r="B11" s="6">
+        <v>45362.49930555555</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="7"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="9"/>
       <c r="G11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="4">
+      <c r="H11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="A12" s="6">
         <v>45362</v>
       </c>
-      <c r="B12" s="4">
-        <v>99783.49930555555</v>
+      <c r="B12" s="6">
+        <v>45362.49930555555</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="9"/>
       <c r="G12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="4">
+      <c r="H12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="6">
         <v>45362</v>
       </c>
-      <c r="B13" s="4">
-        <v>99783.49930555555</v>
+      <c r="B13" s="6">
+        <v>45362.49930555555</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="7"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="9"/>
       <c r="G13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="4">
+      <c r="H13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="6">
         <v>45362</v>
       </c>
-      <c r="B14" s="4">
-        <v>99783.49930555555</v>
+      <c r="B14" s="6">
+        <v>45362.49930555555</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="7"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="9"/>
       <c r="G14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="4">
+      <c r="H14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="6">
         <v>45376</v>
       </c>
-      <c r="B15" s="4">
-        <v>99797.49930555555</v>
+      <c r="B15" s="6">
+        <v>45376.49930555555</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="7"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="9"/>
       <c r="G15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="4">
+      <c r="H15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="6">
         <v>45380</v>
       </c>
-      <c r="B16" s="4">
-        <v>99801.49930555555</v>
+      <c r="B16" s="6">
+        <v>45380.49930555555</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="7"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="9"/>
       <c r="G16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="4">
+      <c r="H16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="6">
         <v>45381</v>
       </c>
-      <c r="B17" s="4">
-        <v>99802.49930555555</v>
+      <c r="B17" s="6">
+        <v>45381.49930555555</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="7"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="9"/>
       <c r="G17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="4">
+      <c r="H17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="6">
         <v>45382</v>
       </c>
-      <c r="B18" s="4">
-        <v>99803.49930555555</v>
+      <c r="B18" s="6">
+        <v>45382.49930555555</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="7"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="9"/>
       <c r="G18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="4">
+      <c r="H18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+      <c r="A19" s="6">
         <v>45383</v>
       </c>
-      <c r="B19" s="4">
-        <v>99804.49930555555</v>
+      <c r="B19" s="6">
+        <v>45383.49930555555</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="7"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="9"/>
       <c r="G19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="4">
+      <c r="H19" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+      <c r="A20" s="6">
         <v>45384</v>
       </c>
-      <c r="B20" s="4">
-        <v>99805.49930555555</v>
+      <c r="B20" s="6">
+        <v>45384.49930555555</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="7"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="9"/>
       <c r="G20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="4">
+      <c r="H20" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+      <c r="A21" s="6">
         <v>45407</v>
       </c>
-      <c r="B21" s="4">
-        <v>99828.49930555555</v>
+      <c r="B21" s="6">
+        <v>45407.49930555555</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="7"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="9"/>
       <c r="G21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="4">
+      <c r="H21" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+      <c r="A22" s="6">
         <v>45418</v>
       </c>
-      <c r="B22" s="4">
-        <v>99839.49930555555</v>
+      <c r="B22" s="6">
+        <v>45418.49930555555</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="6"/>
-      <c r="F22" s="7"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="9"/>
       <c r="G22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="4">
+      <c r="H22" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+      <c r="A23" s="6">
         <v>45418</v>
       </c>
-      <c r="B23" s="4">
-        <v>99839.49930555555</v>
+      <c r="B23" s="6">
+        <v>45418.49930555555</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="6"/>
-      <c r="F23" s="7"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="9"/>
       <c r="G23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="4">
+      <c r="H23" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+      <c r="A24" s="6">
         <v>45439</v>
       </c>
-      <c r="B24" s="4">
-        <v>99860.49930555555</v>
+      <c r="B24" s="6">
+        <v>45439.49930555555</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="7"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="9"/>
       <c r="G24" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H24" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="4">
+      <c r="H24" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+      <c r="A25" s="6">
         <v>45446</v>
       </c>
-      <c r="B25" s="4">
-        <v>99867.49930555555</v>
+      <c r="B25" s="6">
+        <v>45446.49930555555</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="6"/>
-      <c r="F25" s="7"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="9"/>
       <c r="G25" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H25" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="4">
+      <c r="H25" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
+      <c r="A26" s="6">
         <v>45446</v>
       </c>
-      <c r="B26" s="4">
-        <v>99867.49930555555</v>
+      <c r="B26" s="6">
+        <v>45446.49930555555</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E26" s="6"/>
-      <c r="F26" s="7"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="9"/>
       <c r="G26" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H26" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="4">
+      <c r="H26" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
+      <c r="A27" s="6">
         <v>45453</v>
       </c>
-      <c r="B27" s="4">
-        <v>99874.49930555555</v>
+      <c r="B27" s="6">
+        <v>45453.49930555555</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="7"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="9"/>
       <c r="G27" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="4">
+      <c r="H27" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
+      <c r="A28" s="6">
         <v>45509</v>
       </c>
-      <c r="B28" s="4">
-        <v>99930.49930555555</v>
+      <c r="B28" s="6">
+        <v>45509.49930555555</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="6"/>
-      <c r="F28" s="7"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="9"/>
       <c r="G28" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H28" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="4">
+      <c r="H28" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
+      <c r="A29" s="6">
         <v>45518</v>
       </c>
-      <c r="B29" s="4">
-        <v>99939.49930555555</v>
+      <c r="B29" s="6">
+        <v>45518.49930555555</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="7"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="9"/>
       <c r="G29" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H29" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="4">
+      <c r="H29" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
+      <c r="A30" s="6">
         <v>45558</v>
       </c>
-      <c r="B30" s="4">
-        <v>99979.49930555555</v>
+      <c r="B30" s="6">
+        <v>45558.49930555555</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="7"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="9"/>
       <c r="G30" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H30" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="4">
+      <c r="H30" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+      <c r="A31" s="6">
         <v>45572</v>
       </c>
-      <c r="B31" s="4">
-        <v>99993.49930555555</v>
+      <c r="B31" s="6">
+        <v>45572.49930555555</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E31" s="6"/>
-      <c r="F31" s="7"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="9"/>
       <c r="G31" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H31" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="4">
+      <c r="H31" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
+      <c r="A32" s="6">
         <v>45572</v>
       </c>
-      <c r="B32" s="4">
-        <v>99993.49930555555</v>
+      <c r="B32" s="6">
+        <v>45572.49930555555</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E32" s="6"/>
-      <c r="F32" s="7"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="9"/>
       <c r="G32" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H32" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="4">
+      <c r="H32" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+      <c r="A33" s="6">
         <v>45590</v>
       </c>
-      <c r="B33" s="4">
-        <v>100011.49930555555</v>
+      <c r="B33" s="6">
+        <v>45590.49930555555</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E33" s="6"/>
-      <c r="F33" s="7"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="9"/>
       <c r="G33" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H33" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
-      <c r="A34" s="4">
+      <c r="H33" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
+      <c r="A34" s="6">
         <v>45593</v>
       </c>
-      <c r="B34" s="4">
-        <v>100014.49930555555</v>
+      <c r="B34" s="6">
+        <v>45593.49930555555</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E34" s="6"/>
-      <c r="F34" s="7"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="9"/>
       <c r="G34" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H34" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="4">
+      <c r="H34" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
+      <c r="A35" s="6">
         <v>45600</v>
       </c>
-      <c r="B35" s="4">
-        <v>100021.49930555555</v>
+      <c r="B35" s="6">
+        <v>45600.49930555555</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E35" s="6"/>
-      <c r="F35" s="7"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="9"/>
       <c r="G35" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H35" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="4">
+      <c r="H35" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
+      <c r="A36" s="6">
         <v>45600</v>
       </c>
-      <c r="B36" s="4">
-        <v>100021.49930555555</v>
+      <c r="B36" s="6">
+        <v>45600.49930555555</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E36" s="6"/>
-      <c r="F36" s="7"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="9"/>
       <c r="G36" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H36" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
-      <c r="A37" s="4">
+      <c r="H36" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
+      <c r="A37" s="6">
         <v>45601</v>
       </c>
-      <c r="B37" s="4">
-        <v>100022.49930555555</v>
+      <c r="B37" s="6">
+        <v>45601.49930555555</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E37" s="6"/>
-      <c r="F37" s="7"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="9"/>
       <c r="G37" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H37" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
-      <c r="A38" s="4">
+      <c r="H37" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
+      <c r="A38" s="6">
         <v>45611</v>
       </c>
-      <c r="B38" s="4">
-        <v>100032.49930555555</v>
+      <c r="B38" s="6">
+        <v>45611.49930555555</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E38" s="6"/>
-      <c r="F38" s="7"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="9"/>
       <c r="G38" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H38" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="4">
+      <c r="H38" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
+      <c r="A39" s="6">
         <v>45651</v>
       </c>
-      <c r="B39" s="4">
-        <v>100072.49930555555</v>
+      <c r="B39" s="6">
+        <v>45651.49930555555</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E39" s="6"/>
-      <c r="F39" s="7"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="9"/>
       <c r="G39" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H39" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
-      <c r="A40" s="4">
+      <c r="H39" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
+      <c r="A40" s="6">
         <v>45652</v>
       </c>
-      <c r="B40" s="4">
-        <v>100073.49930555555</v>
+      <c r="B40" s="6">
+        <v>45652.49930555555</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E40" s="6"/>
-      <c r="F40" s="7"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="9"/>
       <c r="G40" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H40" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I40" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
-      <c r="A41" s="4">
+      <c r="H40" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
+      <c r="A41" s="6">
         <v>45652</v>
       </c>
-      <c r="B41" s="4">
-        <v>100073.49930555555</v>
+      <c r="B41" s="6">
+        <v>45652.49930555555</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E41" s="6"/>
-      <c r="F41" s="7"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="9"/>
       <c r="G41" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H41" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I41" s="5" t="s">
+      <c r="H41" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I41" s="7" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>